<commit_message>
Complete test case with POM DD framework
</commit_message>
<xml_diff>
--- a/sampleproject/ExcelData/SendingAndVerifyingMail.xlsx
+++ b/sampleproject/ExcelData/SendingAndVerifyingMail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>FromGmailPassword</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>Test gMail-</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +438,7 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>

</xml_diff>